<commit_message>
einige Publication.source ergänzt, editor in editors umbenannt
</commit_message>
<xml_diff>
--- a/MethodDemos/output/statistics/cermine-AUTHORS.xlsx
+++ b/MethodDemos/output/statistics/cermine-AUTHORS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="246">
   <si>
     <t>TUW-137078</t>
   </si>
@@ -35,10 +35,10 @@
   </si>
   <si>
     <t>Marije Geldof
-2Annette ten Teije
-2Frank van Harmelen
-2Mar Marcos
-1Peter Votruba</t>
+Annette ten Teije
+Frank van Harmelen
+Mar Marcos
+Peter Votruba</t>
   </si>
   <si>
     <t>TUW-138447</t>
@@ -80,7 +80,7 @@
   </si>
   <si>
     <t>Univ.-Prof. Dr. Michael Hanke
-0Andreas Heigl</t>
+Andreas Heigl</t>
   </si>
   <si>
     <t>TUW-139769</t>
@@ -128,19 +128,11 @@
 Marco Zapletal</t>
   </si>
   <si>
-    <t>Michael Ilger
-0Marco Zapletal</t>
-  </si>
-  <si>
     <t>TUW-140229</t>
   </si>
   <si>
     <t>Sabine Graf
 Kinshuk</t>
-  </si>
-  <si>
-    <t>Sabine Graf
-1Kinshuk</t>
   </si>
   <si>
     <t>TUW-140253</t>
@@ -183,7 +175,7 @@
   </si>
   <si>
     <t>Steve Cayzer
-012steve.cayzer@hp.com</t>
+steve.cayzer@hp.com</t>
   </si>
   <si>
     <t>TUW-141024</t>
@@ -203,11 +195,6 @@
 Kinshuk</t>
   </si>
   <si>
-    <t>Sabine Graf
-2Taiyu Lin
-1Kinshuk</t>
-  </si>
-  <si>
     <t>TUW-141121</t>
   </si>
   <si>
@@ -216,9 +203,9 @@
   </si>
   <si>
     <t>Robert Neumayer
-0Andreas Rauber
-0neumayer
-0rauber}@ifs.tuwien.ac.at</t>
+Andreas Rauber
+neumayer
+rauber}@ifs.tuwien.ac.at</t>
   </si>
   <si>
     <t>TUW-141140</t>
@@ -247,25 +234,25 @@
   </si>
   <si>
     <t>Antonio Vallecillo
-5Nora Koch
-1Cristina Cachero
-4Sara Comai
-2Piero Fraternali
-2Irene Garrigós
-4Jaime Gómez
-4Gerti Kappel
-3Alexander Knapp
-1Maristella Matera
-2Santiago Meliá
-4Nathalie Moreno
-5Birgit Pröll
-0Thomas Reiter
-0Werner Ret- schitzegger
-0José E. Rivera
-5Andrea Schauerhuber
-3Wieland Schwinger
-0Manuel Wimmer
-3Gefei Zhang</t>
+Nora Koch
+Cristina Cachero
+Sara Comai
+Piero Fraternali
+Irene Garrigós
+Jaime Gómez
+Gerti Kappel
+Alexander Knapp
+Maristella Matera
+Santiago Meliá
+Nathalie Moreno
+Birgit Pröll
+Thomas Reiter
+Werner Ret- schitzegger
+José E. Rivera
+Andrea Schauerhuber
+Wieland Schwinger
+Manuel Wimmer
+Gefei Zhang</t>
   </si>
   <si>
     <t>TUW-141336</t>
@@ -277,13 +264,13 @@
   </si>
   <si>
     <t>Nadia Creignou LIF
-01UMR CNRS
-01Universit´e de la M´editerran´ee
-01avenue de Luminy
-01Marseille
-01France
-01Herv´e Daud´e LATP
-01UMR CNRS</t>
+UMR CNRS
+Universit´e de la M´editerran´ee
+avenue de Luminy
+Marseille
+France
+Herv´e Daud´e LATP
+UMR CNRS</t>
   </si>
   <si>
     <t>TUW-141618</t>
@@ -327,9 +314,9 @@
   </si>
   <si>
     <t>Guenter Kiechle
-2Karl F. Doerner
-1Michel Gendreau
-0Richard F. Hartl</t>
+Karl F. Doerner
+Michel Gendreau
+Richard F. Hartl</t>
   </si>
   <si>
     <t>TUW-172697</t>
@@ -343,14 +330,6 @@
 Andreas Rauber</t>
   </si>
   <si>
-    <t>Hannes Kulovits
-0Christoph Becker
-0Michael Kraxner
-0Florian Motlik
-0Kevin Stadler
-0Andreas Rauber</t>
-  </si>
-  <si>
     <t>TUW-174216</t>
   </si>
   <si>
@@ -362,7 +341,7 @@
   </si>
   <si>
     <t>Christoph Becker
-01Andreas Rauber</t>
+Andreas Rauber</t>
   </si>
   <si>
     <t>TUW-175428</t>
@@ -392,17 +371,17 @@
   </si>
   <si>
     <t>Susana JIMÉNEZ-MURCIA
-0Fernando FERNÁNDEZ-ARANDA
-0Elias KALAPANIDAS
-2Dimitri KONSTANTAS
-3Todor GANCHEV
-5Otilia KOCSIS
-5Tony LAM
-1Juan J. SANTAMARÍA
-0Thierry RAGUIN
-1Christian BREITENEDER
-4Hannes KAUFMANN
-4Costas DAVARAKIS</t>
+Fernando FERNÁNDEZ-ARANDA
+Elias KALAPANIDAS
+Dimitri KONSTANTAS
+Todor GANCHEV
+Otilia KOCSIS
+Tony LAM
+Juan J. SANTAMARÍA
+Thierry RAGUIN
+Christian BREITENEDER
+Hannes KAUFMANN
+Costas DAVARAKIS</t>
   </si>
   <si>
     <t>TUW-177140</t>
@@ -412,12 +391,6 @@
 Martina Seidl
 Hans Tompits
 Stefan Woltran</t>
-  </si>
-  <si>
-    <t>Johannes Oetsch
-0Martina Seidl
-1Hans Tompits
-0Stefan Woltran</t>
   </si>
   <si>
     <t>TUW-179146</t>
@@ -432,7 +405,7 @@
   </si>
   <si>
     <t>Eva Ku¨ hn, Richard Mordinyi,
-0Sandford Bessler, Slobodanka Tomic</t>
+Sandford Bessler, Slobodanka Tomic</t>
   </si>
   <si>
     <t>TUW-180162</t>
@@ -441,11 +414,6 @@
     <t>Manuel Egele
 Christopher Kruegel
 Engin Kirda</t>
-  </si>
-  <si>
-    <t>Manuel Egele
-1Christopher Kruegel
-2Engin Kirda</t>
   </si>
   <si>
     <t>TUW-181199</t>
@@ -459,10 +427,10 @@
   </si>
   <si>
     <t>Martin Gebser
-0Jo¨ rg Pu¨ hrer
-1Torsten Schaub
-0Hans Tompits
-1Stefan Woltran</t>
+Jo¨ rg Pu¨ hrer
+Torsten Schaub
+Hans Tompits
+Stefan Woltran</t>
   </si>
   <si>
     <t>TUW-182414</t>
@@ -473,8 +441,8 @@
   </si>
   <si>
     <t>Andreas Rauber
-1Schlagworte
-2Max Kaiser</t>
+Schlagworte
+Max Kaiser</t>
   </si>
   <si>
     <t>TUW-182899</t>
@@ -482,10 +450,6 @@
   <si>
     <t>Rowanne Fleck
 Geraldine Fitzpatrick</t>
-  </si>
-  <si>
-    <t>Rowanne Fleck
-0Geraldine Fitzpatrick</t>
   </si>
   <si>
     <t>TUW-185321</t>
@@ -532,12 +496,12 @@
   </si>
   <si>
     <t>Madeline Balaam, Lesley
-0Ann-Marie Hughes, Jane
-1Stefan Rennick Egglestone,
-5Penny Probert Smith, Nour
-4Geraldine Fitzpatrick Anna Wilkinson, Sue Mawson
-6Thomas Nind, Ian Ricketts Zoe Robertson
-3ACM Classification Keywords</t>
+Ann-Marie Hughes, Jane
+Stefan Rennick Egglestone,
+Penny Probert Smith, Nour
+Geraldine Fitzpatrick Anna Wilkinson, Sue Mawson
+Thomas Nind, Ian Ricketts Zoe Robertson
+ACM Classification Keywords</t>
   </si>
   <si>
     <t>TUW-191715</t>
@@ -565,13 +529,13 @@
   </si>
   <si>
     <t>G. Athanasopoulos
-1E. Fox
-0Y. Ioannidis
-1G. Kakaletris
-1N. Manola
-1C. Meghini
-4A. Rauber
-3D. Soergel</t>
+E. Fox
+Y. Ioannidis
+G. Kakaletris
+N. Manola
+C. Meghini
+A. Rauber
+D. Soergel</t>
   </si>
   <si>
     <t>TUW-192724</t>
@@ -581,10 +545,6 @@
 Irene Krebs</t>
   </si>
   <si>
-    <t>Justyna Patalas-Maliszewska
-1Irene Krebs</t>
-  </si>
-  <si>
     <t>TUW-194085</t>
   </si>
   <si>
@@ -599,10 +559,6 @@
   <si>
     <t>Bernhard Gramlich
 Felix Schernhammer</t>
-  </si>
-  <si>
-    <t>Bernhard Gramlich
-0Felix Schernhammer</t>
   </si>
   <si>
     <t>TUW-194660</t>
@@ -636,11 +592,6 @@
 Thomas Neubauer</t>
   </si>
   <si>
-    <t>Kresimir Kasal
-0Johannes Heurix
-1Thomas Neubauer</t>
-  </si>
-  <si>
     <t>TUW-198401</t>
   </si>
   <si>
@@ -671,7 +622,7 @@
   </si>
   <si>
     <t>zur Erlangung des akademischen Grades
-01Betreuung</t>
+Betreuung</t>
   </si>
   <si>
     <t>TUW-200748</t>
@@ -687,12 +638,6 @@
 Eun Jung Kim
 Stefan Szeider
 Anders Yeo</t>
-  </si>
-  <si>
-    <t>Gregory Gutin
-0Eun Jung Kim
-0Stefan Szeider
-1Anders Yeo</t>
   </si>
   <si>
     <t>TUW-200950</t>
@@ -708,12 +653,12 @@
   </si>
   <si>
     <t>Michael Fellows
-4Fedor V. Fomin
-1Daniel Lokshtanov
-1Frances Rosamond
-4Saket Saurabh
-12Stefan Szeider
-0Carsten Thomassen</t>
+Fedor V. Fomin
+Daniel Lokshtanov
+Frances Rosamond
+Saket Saurabh
+Stefan Szeider
+Carsten Thomassen</t>
   </si>
   <si>
     <t>TUW-200959</t>
@@ -732,8 +677,8 @@
   </si>
   <si>
     <t>Martin Berlakovich
-0Mario Ruthmair
-0Gu¨nther R. Raidl</t>
+Mario Ruthmair
+Gu¨nther R. Raidl</t>
   </si>
   <si>
     <t>TUW-201160</t>
@@ -744,7 +689,7 @@
   </si>
   <si>
     <t>Markus Leitner
-0Gu¨nther R. Raidl</t>
+Gu¨nther R. Raidl</t>
   </si>
   <si>
     <t>TUW-201167</t>
@@ -756,8 +701,8 @@
   </si>
   <si>
     <t>Mario Ruthmair
-0Andreas Hubmer
-0Gu¨nther R. Raidl</t>
+Andreas Hubmer
+Gu¨nther R. Raidl</t>
   </si>
   <si>
     <t>TUW-201821</t>
@@ -773,7 +718,7 @@
   </si>
   <si>
     <t>DIPLOMARBEIT
-0an der</t>
+an der</t>
   </si>
   <si>
     <t>TUW-202824</t>
@@ -781,12 +726,7 @@
   <si>
     <t>Amirreza Tahamtan
 Rainer Kern
-Min Tjoa</t>
-  </si>
-  <si>
-    <t>Amirreza Tahamtan
-012Rainer Kern
-012A Min Tjoa</t>
+A Min Tjoa</t>
   </si>
   <si>
     <t>TUW-203409</t>
@@ -794,10 +734,6 @@
   <si>
     <t>Viktor Pavlu
 Andreas Krall</t>
-  </si>
-  <si>
-    <t>Viktor Pavlu
-0Andreas Krall</t>
   </si>
   <si>
     <t>TUW-203924</t>
@@ -812,10 +748,10 @@
   </si>
   <si>
     <t>Matthias SAMWALD
-45Holger STENZHORN
-2Michel DUMONTIER
-0M. Scott MARSHALL
-13Joanne LUCIANOg
+Holger STENZHORN
+Michel DUMONTIER
+M. Scott MARSHALL
+Joanne LUCIANOg
 Klaus-Peter ADLASSNIGi</t>
   </si>
   <si>
@@ -834,8 +770,8 @@
   </si>
   <si>
     <t>Jens Knoop
-0Laura Kova´cs
-0Jakob Zwirchmayr??</t>
+Laura Kova´cs
+Jakob Zwirchmayr??</t>
   </si>
   <si>
     <t>TUW-205933</t>
@@ -861,11 +797,11 @@
   </si>
   <si>
     <t>Samwald M
-012Kritz M
-3Gschwandtner M
-3Stefanov V
-1Hanbury A
-1Support, Multilinguality</t>
+Kritz M
+Gschwandtner M
+Stefanov V
+Hanbury A
+Support, Multilinguality</t>
   </si>
   <si>
     <t>TUW-217690</t>
@@ -879,7 +815,7 @@
   </si>
   <si>
     <t>Georg Gerstweiler
-0Christian Schönauer</t>
+Christian Schönauer</t>
   </si>
   <si>
     <t>TUW-217971</t>
@@ -903,20 +839,11 @@
 Manfred Del Fabro</t>
   </si>
   <si>
-    <t>Matthias Zeppelzauer
-2Maia Zaharieva
-1Manfred Del Fabro</t>
-  </si>
-  <si>
     <t>TUW-223973</t>
   </si>
   <si>
     <t>Reinhardt Wenzina
 Katharina Kaiser</t>
-  </si>
-  <si>
-    <t>Reinhardt Wenzina
-0Katharina Kaiser</t>
   </si>
   <si>
     <t>TUW-225252</t>
@@ -929,9 +856,9 @@
   </si>
   <si>
     <t>Benjamin Biesinger
-01Christian Schauer
-01Bin Hu
-01Gunther R. Raidl</t>
+Christian Schauer
+Bin Hu
+Gunther R. Raidl</t>
   </si>
   <si>
     <t>TUW-226000</t>
@@ -944,8 +871,8 @@
   </si>
   <si>
     <t>Christopher MAYER
-0Martin MORANDELL
-0Andreas KUNTNER
+Martin MORANDELL
+Andreas KUNTNER
 Hilda TELLIOGLU</t>
   </si>
   <si>
@@ -956,8 +883,8 @@
   </si>
   <si>
     <t>Computational Intelligence
-0Ioana Jucu Registration Number
-0Advisor: Priv.-Doz. Dr. Laura Kovacs</t>
+Ioana Jucu Registration Number
+Advisor: Priv.-Doz. Dr. Laura Kovacs</t>
   </si>
   <si>
     <t>TUW-228620</t>
@@ -969,12 +896,6 @@
 A Min Tjoa</t>
   </si>
   <si>
-    <t>Sven Wohlgemuth
-0345Stefan Sackmann
-0345Noboru Sonehara
-0345A Min Tjoa</t>
-  </si>
-  <si>
     <t>TUW-231707</t>
   </si>
   <si>
@@ -991,9 +912,9 @@
   </si>
   <si>
     <t>Christian Bors
-0Theresia Gschwandtner
-0Silvia Miksch
-0Johannes Ga¨ rtner</t>
+Theresia Gschwandtner
+Silvia Miksch
+Johannes Ga¨ rtner</t>
   </si>
   <si>
     <t>TUW-233657</t>
@@ -1006,12 +927,12 @@
   </si>
   <si>
     <t>Tim Lammarsch
-0123Member
-0123Wolfgang Aigner
-0123Member
-0123Silvia Miksch
-0123Member
-0123Alexander Rind</t>
+Member
+Wolfgang Aigner
+Member
+Silvia Miksch
+Member
+Alexander Rind</t>
   </si>
   <si>
     <t>TUW-236063</t>
@@ -1032,10 +953,6 @@
 Monika Di Angelo</t>
   </si>
   <si>
-    <t>Markus Brunner
-0Monika Di Angelo</t>
-  </si>
-  <si>
     <t>TUW-237297</t>
   </si>
   <si>
@@ -1050,11 +967,6 @@
 Andreas Pieris</t>
   </si>
   <si>
-    <t>Marco Calautti
-0Georg Gottlob
-1Andreas Pieris</t>
-  </si>
-  <si>
     <t>TUW-245336</t>
   </si>
   <si>
@@ -1069,11 +981,6 @@
 Florina Piroi</t>
   </si>
   <si>
-    <t>Elisabeta Spunei
-0Ion Piroi
-0Florina Piroi</t>
-  </si>
-  <si>
     <t>TUW-247301</t>
   </si>
   <si>
@@ -1082,11 +989,6 @@
 Andreas Pieris</t>
   </si>
   <si>
-    <t>Georg Gottlob
-0Marco Manna
-1Andreas Pieris</t>
-  </si>
-  <si>
     <t>TUW-247741</t>
   </si>
   <si>
@@ -1096,7 +998,7 @@
   </si>
   <si>
     <t>Abdel Aziz Taha
-01Allan Hanbury</t>
+Allan Hanbury</t>
   </si>
   <si>
     <t>TUW-247743</t>
@@ -1106,7 +1008,7 @@
   </si>
   <si>
     <t>unter Anleitung von
-01Taha Abdel Aziz</t>
+Taha Abdel Aziz</t>
   </si>
   <si>
     <t>TUW-251544</t>
@@ -1120,7 +1022,7 @@
   </si>
   <si>
     <t>Bogdan Ionescu
-Alexandru Lucian Gînsc
+Alexandru Lucian Gînscă
 Maia Zaharieva
 Bogdan Boteanu
 Mihai Lupu
@@ -1128,11 +1030,11 @@
   </si>
   <si>
     <t>Bogdan Ionescu
-2Bogdan Boteanu
-2Alexandru Lucian Gînsca˘
-0Mihai Lupu
-4Maia Zaharieva
-3Henning Müller</t>
+Bogdan Boteanu
+Alexandru Lucian Gînsca˘
+Mihai Lupu
+Maia Zaharieva
+Henning Müller</t>
   </si>
   <si>
     <t>TUW-255712</t>
@@ -1165,8 +1067,8 @@
   </si>
   <si>
     <t>Jean D. Hallewell Haslwanter
-2Geraldine Fitzpatrick
-0Author Keywords</t>
+Geraldine Fitzpatrick
+Author Keywords</t>
   </si>
 </sst>
 </file>
@@ -3922,7 +3824,7 @@
     <col min="3" max="3" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="26.578125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="47.5625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="46.44921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="19.921875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="4.9296875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="4.9296875" customWidth="true" bestFit="true"/>
@@ -4264,7 +4166,7 @@
         <v>31</v>
       </c>
       <c r="F12" t="s" s="105">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" t="n" s="106">
         <v>1.0</v>
@@ -4278,7 +4180,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="109">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="110">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-140229.pdf")</f>
@@ -4290,10 +4192,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-140229-xstream.xml")</f>
       </c>
       <c r="E13" t="s" s="113">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s" s="114">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" t="n" s="115">
         <v>1.0</v>
@@ -4307,7 +4209,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="118">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="119">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-140253.pdf")</f>
@@ -4319,10 +4221,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-140253-xstream.xml")</f>
       </c>
       <c r="E14" t="s" s="122">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s" s="123">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G14" t="n" s="124">
         <v>1.0</v>
@@ -4336,7 +4238,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="127">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="128">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-140308.pdf")</f>
@@ -4348,10 +4250,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-140308-xstream.xml")</f>
       </c>
       <c r="E15" t="s" s="131">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s" s="132">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G15" t="n" s="133">
         <v>1.0</v>
@@ -4365,7 +4267,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="136">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="137">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-140533.pdf")</f>
@@ -4377,7 +4279,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-140533-xstream.xml")</f>
       </c>
       <c r="E16" t="s" s="140">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s" s="141">
         <v>21</v>
@@ -4394,7 +4296,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="145">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="146">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-140867.pdf")</f>
@@ -4406,7 +4308,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-140867-xstream.xml")</f>
       </c>
       <c r="E17" t="s" s="149">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s" s="150">
         <v>11</v>
@@ -4423,7 +4325,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="154">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="155">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-140895.pdf")</f>
@@ -4435,7 +4337,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-140895-xstream.xml")</f>
       </c>
       <c r="E18" t="s" s="158">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s" s="159">
         <v>21</v>
@@ -4452,7 +4354,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="163">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="164">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-140983.pdf")</f>
@@ -4464,10 +4366,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-140983-xstream.xml")</f>
       </c>
       <c r="E19" t="s" s="167">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s" s="168">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G19" t="n" s="169">
         <v>0.5</v>
@@ -4481,7 +4383,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="172">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="173">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-141024.pdf")</f>
@@ -4493,7 +4395,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-141024-xstream.xml")</f>
       </c>
       <c r="E20" t="s" s="176">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s" s="177">
         <v>11</v>
@@ -4510,7 +4412,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="181">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="182">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-141065.pdf")</f>
@@ -4522,10 +4424,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-141065-xstream.xml")</f>
       </c>
       <c r="E21" t="s" s="185">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s" s="186">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G21" t="n" s="187">
         <v>1.0</v>
@@ -4539,7 +4441,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="190">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" s="191">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-141121.pdf")</f>
@@ -4551,10 +4453,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-141121-xstream.xml")</f>
       </c>
       <c r="E22" t="s" s="194">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s" s="195">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G22" t="n" s="196">
         <v>0.5</v>
@@ -4568,7 +4470,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="199">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B23" s="200">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-141140.pdf")</f>
@@ -4580,10 +4482,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-141140-xstream.xml")</f>
       </c>
       <c r="E23" t="s" s="203">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s" s="204">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G23" t="n" s="205">
         <v>1.0</v>
@@ -4597,7 +4499,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="208">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B24" s="209">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-141336.pdf")</f>
@@ -4609,10 +4511,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-141336-xstream.xml")</f>
       </c>
       <c r="E24" t="s" s="212">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s" s="213">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G24" t="n" s="214">
         <v>0.0</v>
@@ -4626,7 +4528,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="217">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B25" s="218">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-141618.pdf")</f>
@@ -4638,7 +4540,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-141618-xstream.xml")</f>
       </c>
       <c r="E25" t="s" s="221">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s" s="222">
         <v>11</v>
@@ -4655,7 +4557,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="226">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" s="227">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-141758.pdf")</f>
@@ -4667,7 +4569,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-141758-xstream.xml")</f>
       </c>
       <c r="E26" t="s" s="230">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F26" t="s" s="231">
         <v>11</v>
@@ -4684,7 +4586,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="235">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B27" s="236">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-168222.pdf")</f>
@@ -4696,7 +4598,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-168222-xstream.xml")</f>
       </c>
       <c r="E27" t="s" s="239">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s" s="240">
         <v>11</v>
@@ -4713,7 +4615,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="244">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B28" s="245">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-168482.pdf")</f>
@@ -4725,10 +4627,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-168482-xstream.xml")</f>
       </c>
       <c r="E28" t="s" s="248">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F28" t="s" s="249">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G28" t="n" s="250">
         <v>0.0</v>
@@ -4742,7 +4644,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="253">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B29" s="254">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-169511.pdf")</f>
@@ -4754,10 +4656,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-169511-xstream.xml")</f>
       </c>
       <c r="E29" t="s" s="257">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F29" t="s" s="258">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G29" t="n" s="259">
         <v>1.0</v>
@@ -4771,7 +4673,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="262">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B30" s="263">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-172697.pdf")</f>
@@ -4783,10 +4685,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-172697-xstream.xml")</f>
       </c>
       <c r="E30" t="s" s="266">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F30" t="s" s="267">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G30" t="n" s="268">
         <v>1.0</v>
@@ -4800,7 +4702,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="271">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B31" s="272">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-174216.pdf")</f>
@@ -4812,10 +4714,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-174216-xstream.xml")</f>
       </c>
       <c r="E31" t="s" s="275">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F31" t="s" s="276">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G31" t="n" s="277">
         <v>1.0</v>
@@ -4829,7 +4731,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="280">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B32" s="281">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-175428.pdf")</f>
@@ -4841,10 +4743,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-175428-xstream.xml")</f>
       </c>
       <c r="E32" t="s" s="284">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s" s="285">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G32" t="n" s="286">
         <v>0.0</v>
@@ -4858,7 +4760,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="289">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B33" s="290">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-176087.pdf")</f>
@@ -4870,10 +4772,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-176087-xstream.xml")</f>
       </c>
       <c r="E33" t="s" s="293">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F33" t="s" s="294">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G33" t="n" s="295">
         <v>1.0</v>
@@ -4887,7 +4789,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="298">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B34" s="299">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-177140.pdf")</f>
@@ -4899,10 +4801,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-177140-xstream.xml")</f>
       </c>
       <c r="E34" t="s" s="302">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F34" t="s" s="303">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G34" t="n" s="304">
         <v>1.0</v>
@@ -4916,7 +4818,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="307">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B35" s="308">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-179146.pdf")</f>
@@ -4928,10 +4830,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-179146-xstream.xml")</f>
       </c>
       <c r="E35" t="s" s="311">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s" s="312">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G35" t="n" s="313">
         <v>0.0</v>
@@ -4945,7 +4847,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="316">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B36" s="317">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-180162.pdf")</f>
@@ -4957,10 +4859,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-180162-xstream.xml")</f>
       </c>
       <c r="E36" t="s" s="320">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F36" t="s" s="321">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G36" t="n" s="322">
         <v>1.0</v>
@@ -4974,7 +4876,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="325">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B37" s="326">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-181199.pdf")</f>
@@ -4986,10 +4888,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-181199-xstream.xml")</f>
       </c>
       <c r="E37" t="s" s="329">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F37" t="s" s="330">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G37" t="n" s="331">
         <v>0.8</v>
@@ -5003,7 +4905,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="334">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B38" s="335">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-182414.pdf")</f>
@@ -5015,10 +4917,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-182414-xstream.xml")</f>
       </c>
       <c r="E38" t="s" s="338">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s" s="339">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G38" t="n" s="340">
         <v>0.67</v>
@@ -5032,7 +4934,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="343">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B39" s="344">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-182899.pdf")</f>
@@ -5044,10 +4946,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-182899-xstream.xml")</f>
       </c>
       <c r="E39" t="s" s="347">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F39" t="s" s="348">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G39" t="n" s="349">
         <v>1.0</v>
@@ -5061,7 +4963,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="352">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B40" s="353">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-185321.pdf")</f>
@@ -5073,7 +4975,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-185321-xstream.xml")</f>
       </c>
       <c r="E40" t="s" s="356">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F40" t="s" s="357">
         <v>11</v>
@@ -5090,7 +4992,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="361">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B41" s="362">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-185441.pdf")</f>
@@ -5102,7 +5004,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-185441-xstream.xml")</f>
       </c>
       <c r="E41" t="s" s="365">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F41" t="s" s="366">
         <v>11</v>
@@ -5119,7 +5021,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="370">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B42" s="371">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-186227.pdf")</f>
@@ -5131,7 +5033,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-186227-xstream.xml")</f>
       </c>
       <c r="E42" t="s" s="374">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F42" t="s" s="375">
         <v>11</v>
@@ -5148,7 +5050,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="379">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B43" s="380">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-189842.pdf")</f>
@@ -5160,10 +5062,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-189842-xstream.xml")</f>
       </c>
       <c r="E43" t="s" s="383">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F43" t="s" s="384">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G43" t="n" s="385">
         <v>0.14</v>
@@ -5177,7 +5079,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="388">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B44" s="389">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-191715.pdf")</f>
@@ -5189,10 +5091,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-191715-xstream.xml")</f>
       </c>
       <c r="E44" t="s" s="392">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F44" t="s" s="393">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G44" t="n" s="394">
         <v>1.0</v>
@@ -5206,7 +5108,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="397">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B45" s="398">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-191977.pdf")</f>
@@ -5218,10 +5120,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-191977-xstream.xml")</f>
       </c>
       <c r="E45" t="s" s="401">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F45" t="s" s="402">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G45" t="n" s="403">
         <v>1.0</v>
@@ -5235,7 +5137,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="406">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B46" s="407">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-192724.pdf")</f>
@@ -5247,10 +5149,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-192724-xstream.xml")</f>
       </c>
       <c r="E46" t="s" s="410">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F46" t="s" s="411">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G46" t="n" s="412">
         <v>1.0</v>
@@ -5264,7 +5166,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="415">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B47" s="416">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-194085.pdf")</f>
@@ -5276,10 +5178,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-194085-xstream.xml")</f>
       </c>
       <c r="E47" t="s" s="419">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F47" t="s" s="420">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G47" t="n" s="421">
         <v>0.0</v>
@@ -5293,7 +5195,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="424">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B48" s="425">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-194561.pdf")</f>
@@ -5305,10 +5207,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-194561-xstream.xml")</f>
       </c>
       <c r="E48" t="s" s="428">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F48" t="s" s="429">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G48" t="n" s="430">
         <v>1.0</v>
@@ -5322,7 +5224,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="433">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B49" s="434">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-194660.pdf")</f>
@@ -5334,7 +5236,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-194660-xstream.xml")</f>
       </c>
       <c r="E49" t="s" s="437">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F49" t="s" s="438">
         <v>11</v>
@@ -5351,7 +5253,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="442">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B50" s="443">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-197422.pdf")</f>
@@ -5363,10 +5265,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-197422-xstream.xml")</f>
       </c>
       <c r="E50" t="s" s="446">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F50" t="s" s="447">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G50" t="n" s="448">
         <v>1.0</v>
@@ -5380,7 +5282,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="451">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B51" s="452">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-197852.pdf")</f>
@@ -5392,7 +5294,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-197852-xstream.xml")</f>
       </c>
       <c r="E51" t="s" s="455">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F51" t="s" s="456">
         <v>11</v>
@@ -5409,7 +5311,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="460">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B52" s="461">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-198400.pdf")</f>
@@ -5421,10 +5323,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-198400-xstream.xml")</f>
       </c>
       <c r="E52" t="s" s="464">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F52" t="s" s="465">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="G52" t="n" s="466">
         <v>1.0</v>
@@ -5438,7 +5340,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="469">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B53" s="470">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-198401.pdf")</f>
@@ -5450,7 +5352,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-198401-xstream.xml")</f>
       </c>
       <c r="E53" t="s" s="473">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F53" t="s" s="474">
         <v>11</v>
@@ -5467,7 +5369,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="478">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B54" s="479">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-198405.pdf")</f>
@@ -5479,7 +5381,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-198405-xstream.xml")</f>
       </c>
       <c r="E54" t="s" s="482">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F54" t="s" s="483">
         <v>11</v>
@@ -5496,7 +5398,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="487">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B55" s="488">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-198408.pdf")</f>
@@ -5508,10 +5410,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-198408-xstream.xml")</f>
       </c>
       <c r="E55" t="s" s="491">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F55" t="s" s="492">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="G55" t="n" s="493">
         <v>0.0</v>
@@ -5525,7 +5427,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="496">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B56" s="497">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-200745.pdf")</f>
@@ -5537,10 +5439,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-200745-xstream.xml")</f>
       </c>
       <c r="E56" t="s" s="500">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F56" t="s" s="501">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="G56" t="n" s="502">
         <v>0.0</v>
@@ -5554,7 +5456,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="505">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B57" s="506">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-200748.pdf")</f>
@@ -5566,10 +5468,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-200748-xstream.xml")</f>
       </c>
       <c r="E57" t="s" s="509">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F57" t="s" s="510">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G57" t="n" s="511">
         <v>0.0</v>
@@ -5583,7 +5485,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="514">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B58" s="515">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-200948.pdf")</f>
@@ -5595,10 +5497,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-200948-xstream.xml")</f>
       </c>
       <c r="E58" t="s" s="518">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F58" t="s" s="519">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G58" t="n" s="520">
         <v>1.0</v>
@@ -5612,7 +5514,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="523">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B59" s="524">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-200950.pdf")</f>
@@ -5624,10 +5526,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-200950-xstream.xml")</f>
       </c>
       <c r="E59" t="s" s="527">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F59" t="s" s="528">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G59" t="n" s="529">
         <v>1.0</v>
@@ -5641,7 +5543,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="532">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B60" s="533">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-200959.pdf")</f>
@@ -5653,7 +5555,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-200959-xstream.xml")</f>
       </c>
       <c r="E60" t="s" s="536">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="F60" t="s" s="537">
         <v>11</v>
@@ -5670,7 +5572,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="541">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B61" s="542">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-201066.pdf")</f>
@@ -5682,10 +5584,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-201066-xstream.xml")</f>
       </c>
       <c r="E61" t="s" s="545">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F61" t="s" s="546">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="G61" t="n" s="547">
         <v>0.67</v>
@@ -5699,7 +5601,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="550">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B62" s="551">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-201160.pdf")</f>
@@ -5711,10 +5613,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-201160-xstream.xml")</f>
       </c>
       <c r="E62" t="s" s="554">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F62" t="s" s="555">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G62" t="n" s="556">
         <v>0.5</v>
@@ -5728,7 +5630,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="559">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B63" s="560">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-201167.pdf")</f>
@@ -5740,10 +5642,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-201167-xstream.xml")</f>
       </c>
       <c r="E63" t="s" s="563">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="F63" t="s" s="564">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="G63" t="n" s="565">
         <v>0.67</v>
@@ -5757,7 +5659,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="568">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B64" s="569">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-201821.pdf")</f>
@@ -5769,10 +5671,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-201821-xstream.xml")</f>
       </c>
       <c r="E64" t="s" s="572">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F64" t="s" s="573">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="G64" t="n" s="574">
         <v>1.0</v>
@@ -5786,7 +5688,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="577">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B65" s="578">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-202034.pdf")</f>
@@ -5798,10 +5700,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-202034-xstream.xml")</f>
       </c>
       <c r="E65" t="s" s="581">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F65" t="s" s="582">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="G65" t="n" s="583">
         <v>0.0</v>
@@ -5815,7 +5717,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="586">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B66" s="587">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-202824.pdf")</f>
@@ -5827,24 +5729,24 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-202824-xstream.xml")</f>
       </c>
       <c r="E66" t="s" s="590">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="F66" t="s" s="591">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="G66" t="n" s="592">
-        <v>0.67</v>
+        <v>1.0</v>
       </c>
       <c r="H66" t="n" s="593">
-        <v>0.67</v>
+        <v>1.0</v>
       </c>
       <c r="I66" t="n" s="594">
-        <v>0.67</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="595">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B67" s="596">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-203409.pdf")</f>
@@ -5856,10 +5758,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-203409-xstream.xml")</f>
       </c>
       <c r="E67" t="s" s="599">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F67" t="s" s="600">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G67" t="n" s="601">
         <v>1.0</v>
@@ -5873,7 +5775,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="604">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="B68" s="605">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-203924.pdf")</f>
@@ -5885,10 +5787,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-203924-xstream.xml")</f>
       </c>
       <c r="E68" t="s" s="608">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="F68" t="s" s="609">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="G68" t="n" s="610">
         <v>0.67</v>
@@ -5902,7 +5804,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="613">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B69" s="614">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-204724.pdf")</f>
@@ -5914,10 +5816,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-204724-xstream.xml")</f>
       </c>
       <c r="E69" t="s" s="617">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F69" t="s" s="618">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="G69" t="n" s="619">
         <v>1.0</v>
@@ -5931,7 +5833,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="622">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B70" s="623">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-205557.pdf")</f>
@@ -5943,10 +5845,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-205557-xstream.xml")</f>
       </c>
       <c r="E70" t="s" s="626">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="F70" t="s" s="627">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="G70" t="n" s="628">
         <v>0.67</v>
@@ -5960,7 +5862,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="631">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B71" s="632">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-205933.pdf")</f>
@@ -5972,7 +5874,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-205933-xstream.xml")</f>
       </c>
       <c r="E71" t="s" s="635">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="F71" t="s" s="636">
         <v>11</v>
@@ -5989,7 +5891,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="640">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B72" s="641">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-213513.pdf")</f>
@@ -6001,10 +5903,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-213513-xstream.xml")</f>
       </c>
       <c r="E72" t="s" s="644">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="F72" t="s" s="645">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="G72" t="n" s="646">
         <v>1.0</v>
@@ -6018,7 +5920,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="649">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B73" s="650">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-216744.pdf")</f>
@@ -6030,10 +5932,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-216744-xstream.xml")</f>
       </c>
       <c r="E73" t="s" s="653">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="F73" t="s" s="654">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="G73" t="n" s="655">
         <v>0.0</v>
@@ -6047,7 +5949,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="658">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B74" s="659">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-217690.pdf")</f>
@@ -6059,10 +5961,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-217690-xstream.xml")</f>
       </c>
       <c r="E74" t="s" s="662">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="F74" t="s" s="663">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G74" t="n" s="664">
         <v>1.0</v>
@@ -6076,7 +5978,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="667">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B75" s="668">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-217971.pdf")</f>
@@ -6088,10 +5990,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-217971-xstream.xml")</f>
       </c>
       <c r="E75" t="s" s="671">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="F75" t="s" s="672">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G75" t="n" s="673">
         <v>1.0</v>
@@ -6105,7 +6007,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="676">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B76" s="677">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-221215.pdf")</f>
@@ -6117,10 +6019,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-221215-xstream.xml")</f>
       </c>
       <c r="E76" t="s" s="680">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="F76" t="s" s="681">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G76" t="n" s="682">
         <v>0.0</v>
@@ -6134,7 +6036,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="685">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B77" s="686">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-223906.pdf")</f>
@@ -6146,10 +6048,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-223906-xstream.xml")</f>
       </c>
       <c r="E77" t="s" s="689">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="F77" t="s" s="690">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="G77" t="n" s="691">
         <v>1.0</v>
@@ -6163,7 +6065,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="694">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B78" s="695">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-223973.pdf")</f>
@@ -6175,10 +6077,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-223973-xstream.xml")</f>
       </c>
       <c r="E78" t="s" s="698">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="F78" t="s" s="699">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="G78" t="n" s="700">
         <v>1.0</v>
@@ -6192,7 +6094,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="703">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="B79" s="704">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-225252.pdf")</f>
@@ -6204,10 +6106,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-225252-xstream.xml")</f>
       </c>
       <c r="E79" t="s" s="707">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="F79" t="s" s="708">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="G79" t="n" s="709">
         <v>0.75</v>
@@ -6221,7 +6123,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="712">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B80" s="713">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-226000.pdf")</f>
@@ -6233,10 +6135,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-226000-xstream.xml")</f>
       </c>
       <c r="E80" t="s" s="716">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="F80" t="s" s="717">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="G80" t="n" s="718">
         <v>1.0</v>
@@ -6250,7 +6152,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="721">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="B81" s="722">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-226016.pdf")</f>
@@ -6262,10 +6164,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-226016-xstream.xml")</f>
       </c>
       <c r="E81" t="s" s="725">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="F81" t="s" s="726">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="G81" t="n" s="727">
         <v>0.0</v>
@@ -6279,7 +6181,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="730">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="B82" s="731">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-228620.pdf")</f>
@@ -6291,10 +6193,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-228620-xstream.xml")</f>
       </c>
       <c r="E82" t="s" s="734">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="F82" t="s" s="735">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="G82" t="n" s="736">
         <v>1.0</v>
@@ -6308,7 +6210,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="739">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="B83" s="740">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-231707.pdf")</f>
@@ -6320,10 +6222,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-231707-xstream.xml")</f>
       </c>
       <c r="E83" t="s" s="743">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="F83" t="s" s="744">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="G83" t="n" s="745">
         <v>1.0</v>
@@ -6337,7 +6239,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="748">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="B84" s="749">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-233317.pdf")</f>
@@ -6349,10 +6251,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-233317-xstream.xml")</f>
       </c>
       <c r="E84" t="s" s="752">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="F84" t="s" s="753">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="G84" t="n" s="754">
         <v>0.75</v>
@@ -6366,7 +6268,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="757">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B85" s="758">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-233657.pdf")</f>
@@ -6378,10 +6280,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-233657-xstream.xml")</f>
       </c>
       <c r="E85" t="s" s="761">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="F85" t="s" s="762">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="G85" t="n" s="763">
         <v>0.57</v>
@@ -6395,7 +6297,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="766">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B86" s="767">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-236063.pdf")</f>
@@ -6407,7 +6309,7 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-236063-xstream.xml")</f>
       </c>
       <c r="E86" t="s" s="770">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="F86" t="s" s="771">
         <v>11</v>
@@ -6424,7 +6326,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="775">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="B87" s="776">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-236120.pdf")</f>
@@ -6436,10 +6338,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-236120-xstream.xml")</f>
       </c>
       <c r="E87" t="s" s="779">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="F87" t="s" s="780">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="G87" t="n" s="781">
         <v>1.0</v>
@@ -6453,7 +6355,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="784">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="B88" s="785">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-237297.pdf")</f>
@@ -6465,10 +6367,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-237297-xstream.xml")</f>
       </c>
       <c r="E88" t="s" s="788">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F88" t="s" s="789">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="G88" t="n" s="790">
         <v>1.0</v>
@@ -6482,7 +6384,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="793">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="B89" s="794">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-240858.pdf")</f>
@@ -6494,10 +6396,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-240858-xstream.xml")</f>
       </c>
       <c r="E89" t="s" s="797">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="F89" t="s" s="798">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="G89" t="n" s="799">
         <v>1.0</v>
@@ -6511,7 +6413,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="802">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="B90" s="803">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-245336.pdf")</f>
@@ -6523,10 +6425,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-245336-xstream.xml")</f>
       </c>
       <c r="E90" t="s" s="806">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="F90" t="s" s="807">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="G90" t="n" s="808">
         <v>1.0</v>
@@ -6540,7 +6442,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="811">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="B91" s="812">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-245799.pdf")</f>
@@ -6552,10 +6454,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-245799-xstream.xml")</f>
       </c>
       <c r="E91" t="s" s="815">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="F91" t="s" s="816">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="G91" t="n" s="817">
         <v>1.0</v>
@@ -6569,7 +6471,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="820">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="B92" s="821">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-247301.pdf")</f>
@@ -6581,10 +6483,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-247301-xstream.xml")</f>
       </c>
       <c r="E92" t="s" s="824">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="F92" t="s" s="825">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="G92" t="n" s="826">
         <v>1.0</v>
@@ -6598,7 +6500,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="829">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B93" s="830">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-247741.pdf")</f>
@@ -6610,10 +6512,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-247741-xstream.xml")</f>
       </c>
       <c r="E93" t="s" s="833">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="F93" t="s" s="834">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="G93" t="n" s="835">
         <v>1.0</v>
@@ -6627,7 +6529,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="838">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="B94" s="839">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-247743.pdf")</f>
@@ -6639,10 +6541,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-247743-xstream.xml")</f>
       </c>
       <c r="E94" t="s" s="842">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="F94" t="s" s="843">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="G94" t="n" s="844">
         <v>0.5</v>
@@ -6656,7 +6558,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="847">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="B95" s="848">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-251544.pdf")</f>
@@ -6668,10 +6570,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-251544-xstream.xml")</f>
       </c>
       <c r="E95" t="s" s="851">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="F95" t="s" s="852">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="G95" t="n" s="853">
         <v>1.0</v>
@@ -6685,7 +6587,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="856">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="B96" s="857">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-252847.pdf")</f>
@@ -6697,10 +6599,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-252847-xstream.xml")</f>
       </c>
       <c r="E96" t="s" s="860">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="F96" t="s" s="861">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="G96" t="n" s="862">
         <v>0.83</v>
@@ -6714,7 +6616,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="865">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B97" s="866">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-255712.pdf")</f>
@@ -6726,10 +6628,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-255712-xstream.xml")</f>
       </c>
       <c r="E97" t="s" s="869">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="F97" t="s" s="870">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="G97" t="n" s="871">
         <v>1.0</v>
@@ -6743,7 +6645,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="874">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B98" s="875">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-256654.pdf")</f>
@@ -6755,10 +6657,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-256654-xstream.xml")</f>
       </c>
       <c r="E98" t="s" s="878">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="F98" t="s" s="879">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="G98" t="n" s="880">
         <v>0.5</v>
@@ -6772,7 +6674,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="883">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="B99" s="884">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-257397.pdf")</f>
@@ -6784,10 +6686,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-257397-xstream.xml")</f>
       </c>
       <c r="E99" t="s" s="887">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="F99" t="s" s="888">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="G99" t="n" s="889">
         <v>1.0</v>
@@ -6801,7 +6703,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="892">
-        <v>263</v>
+        <v>243</v>
       </c>
       <c r="B100" s="893">
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\groundtruth\TUW-257870.pdf")</f>
@@ -6813,10 +6715,10 @@
         <f>HYPERLINK("D:\Java\git\MethodDemosGit\MethodDemos\output\extracted\cermine\cermine-TUW-257870-xstream.xml")</f>
       </c>
       <c r="E100" t="s" s="896">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="F100" t="s" s="897">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="G100" t="n" s="898">
         <v>0.67</v>

</xml_diff>